<commit_message>
Not sure this file has actually changed?
</commit_message>
<xml_diff>
--- a/time_shift/original_data/Time shift assays.xlsx
+++ b/time_shift/original_data/Time shift assays.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Dropbox\ESI\MRes\S. thermo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcommon/Documents/OneDrive - University of Exeter/Data/Dan_Coevo/time_shift/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_9AEB870C904FB2646D63A9DD7D61C5E7FFF6D2AF" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4700" yWindow="620" windowWidth="28800" windowHeight="12220" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2.1" sheetId="11" r:id="rId1"/>
@@ -24,9 +23,15 @@
     <sheet name="Mean Phage Infectivity" sheetId="17" r:id="rId9"/>
     <sheet name="Spacer Aquisition" sheetId="18" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="179016" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -126,8 +131,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +195,22 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,11 +278,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -361,19 +384,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -399,9 +424,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -442,6 +467,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -516,13 +542,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.13957190199648731</c:v>
+                    <c:v>0.139571901996487</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.16437934114861913</c:v>
+                    <c:v>0.164379341148619</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.14291201614205964</c:v>
+                    <c:v>0.14291201614206</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -534,13 +560,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.13957190199648731</c:v>
+                    <c:v>0.139571901996487</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.16437934114861913</c:v>
+                    <c:v>0.164379341148619</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.14291201614205964</c:v>
+                    <c:v>0.14291201614206</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -583,19 +609,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.20370370370370372</c:v>
+                  <c:v>0.203703703703704</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52314814814814814</c:v>
+                  <c:v>0.523148148148148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58101851851851849</c:v>
+                  <c:v>0.581018518518518</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-080A-4B56-941A-66DC3AAD81B1}"/>
             </c:ext>
@@ -611,11 +637,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1698900272"/>
-        <c:axId val="1698905168"/>
+        <c:axId val="-160870256"/>
+        <c:axId val="-130105568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1698900272"/>
+        <c:axId val="-160870256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1698905168"/>
+        <c:crossAx val="-130105568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -666,7 +692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1698905168"/>
+        <c:axId val="-130105568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1698900272"/>
+        <c:crossAx val="-160870256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1329,7 +1355,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1370,7 +1396,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1414,7 +1440,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1458,7 +1484,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1502,7 +1528,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1546,7 +1572,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1590,7 +1616,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1634,7 +1660,7 @@
         <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1678,7 +1704,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2003,23 +2029,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="BA17" sqref="BA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="6"/>
-    <col min="2" max="3" width="3.765625" style="6" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="6" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="6" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="6" customWidth="1"/>
-    <col min="30" max="41" width="3.8984375" style="6" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="6"/>
+    <col min="1" max="1" width="9.1640625" style="6"/>
+    <col min="2" max="3" width="3.83203125" style="6" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="6" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="6" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="6" customWidth="1"/>
+    <col min="30" max="41" width="3.83203125" style="6" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -6485,27 +6511,27 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BI108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="AL36" sqref="AL36:AN47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="21"/>
-    <col min="2" max="2" width="4.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="8.47265625" style="21" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="21" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="21"/>
-    <col min="17" max="28" width="3.8984375" style="21" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="21"/>
-    <col min="30" max="41" width="3.8984375" style="21" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="21"/>
+    <col min="1" max="1" width="9.1640625" style="21"/>
+    <col min="2" max="2" width="4.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="21" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="21" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="21"/>
+    <col min="17" max="28" width="3.83203125" style="21" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="21"/>
+    <col min="30" max="41" width="3.83203125" style="21" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:61" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:61" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
       <c r="C3" s="45" t="s">
         <v>23</v>
@@ -6549,52 +6575,52 @@
       <c r="AN3" s="45"/>
       <c r="AO3" s="45"/>
     </row>
-    <row r="4" spans="1:61" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:61" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25"/>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
       <c r="P4" s="19"/>
-      <c r="Q4" s="43" t="s">
+      <c r="Q4" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
       <c r="AC4" s="19"/>
-      <c r="AD4" s="43" t="s">
+      <c r="AD4" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="43"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="43"/>
-      <c r="AK4" s="43"/>
-      <c r="AL4" s="43"/>
-      <c r="AM4" s="43"/>
-      <c r="AN4" s="43"/>
-      <c r="AO4" s="43"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="44"/>
+      <c r="AH4" s="44"/>
+      <c r="AI4" s="44"/>
+      <c r="AJ4" s="44"/>
+      <c r="AK4" s="44"/>
+      <c r="AL4" s="44"/>
+      <c r="AM4" s="44"/>
+      <c r="AN4" s="44"/>
+      <c r="AO4" s="44"/>
       <c r="AS4" s="21">
         <v>2.1</v>
       </c>
@@ -7541,7 +7567,7 @@
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
     </row>
-    <row r="15" spans="1:61" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61" ht="24" x14ac:dyDescent="0.3">
       <c r="B15" s="25"/>
       <c r="C15" s="45" t="s">
         <v>24</v>
@@ -7585,52 +7611,52 @@
       <c r="AN15" s="45"/>
       <c r="AO15" s="45"/>
     </row>
-    <row r="16" spans="1:61" ht="21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="25"/>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
       <c r="P16" s="19"/>
-      <c r="Q16" s="43" t="s">
+      <c r="Q16" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="43"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="43"/>
-      <c r="X16" s="43"/>
-      <c r="Y16" s="43"/>
-      <c r="Z16" s="43"/>
-      <c r="AA16" s="43"/>
-      <c r="AB16" s="43"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="44"/>
+      <c r="X16" s="44"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="44"/>
+      <c r="AA16" s="44"/>
+      <c r="AB16" s="44"/>
       <c r="AC16" s="19"/>
-      <c r="AD16" s="43" t="s">
+      <c r="AD16" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="AE16" s="43"/>
-      <c r="AF16" s="43"/>
-      <c r="AG16" s="43"/>
-      <c r="AH16" s="43"/>
-      <c r="AI16" s="43"/>
-      <c r="AJ16" s="43"/>
-      <c r="AK16" s="43"/>
-      <c r="AL16" s="43"/>
-      <c r="AM16" s="43"/>
-      <c r="AN16" s="43"/>
-      <c r="AO16" s="43"/>
+      <c r="AE16" s="44"/>
+      <c r="AF16" s="44"/>
+      <c r="AG16" s="44"/>
+      <c r="AH16" s="44"/>
+      <c r="AI16" s="44"/>
+      <c r="AJ16" s="44"/>
+      <c r="AK16" s="44"/>
+      <c r="AL16" s="44"/>
+      <c r="AM16" s="44"/>
+      <c r="AN16" s="44"/>
+      <c r="AO16" s="44"/>
     </row>
     <row r="17" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B17" s="25"/>
@@ -8923,23 +8949,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="4"/>
-    <col min="2" max="3" width="3.765625" style="4" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="4" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="4" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="4"/>
-    <col min="30" max="41" width="3.8984375" style="4" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="4"/>
+    <col min="1" max="1" width="9.1640625" style="4"/>
+    <col min="2" max="3" width="3.83203125" style="4" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="4" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="4"/>
+    <col min="30" max="41" width="3.83203125" style="4" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -13620,23 +13646,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="AD31" sqref="AD31:AO42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="4"/>
-    <col min="2" max="3" width="3.765625" style="4" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="4" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="4" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="4"/>
-    <col min="30" max="41" width="3.8984375" style="4" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="4"/>
+    <col min="1" max="1" width="9.1640625" style="4"/>
+    <col min="2" max="3" width="3.83203125" style="4" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="4" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="4"/>
+    <col min="30" max="41" width="3.83203125" style="4" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -18226,23 +18252,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="6"/>
-    <col min="2" max="3" width="3.765625" style="6" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="6" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="6" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="6"/>
-    <col min="30" max="41" width="3.8984375" style="6" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="6"/>
+    <col min="1" max="1" width="9.1640625" style="6"/>
+    <col min="2" max="3" width="3.83203125" style="6" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="6" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="6" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="6"/>
+    <col min="30" max="41" width="3.83203125" style="6" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -22704,23 +22730,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="AU33" sqref="AU33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="12"/>
-    <col min="2" max="3" width="3.765625" style="12" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="13" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="12" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="12" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="12"/>
-    <col min="30" max="41" width="3.8984375" style="12" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="12"/>
+    <col min="1" max="1" width="9.1640625" style="12"/>
+    <col min="2" max="3" width="3.83203125" style="12" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="13" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="12" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="12" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="12"/>
+    <col min="30" max="41" width="3.83203125" style="12" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="12"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -27074,23 +27100,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="10"/>
-    <col min="2" max="3" width="3.765625" style="10" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="11" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="10" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="10" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="10"/>
-    <col min="30" max="41" width="3.8984375" style="10" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="10"/>
+    <col min="1" max="1" width="9.1640625" style="10"/>
+    <col min="2" max="3" width="3.83203125" style="10" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="10" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="10" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="10"/>
+    <col min="30" max="41" width="3.83203125" style="10" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="10"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -31551,23 +31577,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="AD31" sqref="AD31:AO42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="14"/>
-    <col min="2" max="3" width="3.765625" style="14" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="15" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="14" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="14" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="14"/>
-    <col min="30" max="41" width="3.8984375" style="14" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="14"/>
+    <col min="1" max="1" width="9.1640625" style="14"/>
+    <col min="2" max="3" width="3.83203125" style="14" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="15" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="14" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="14" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="14"/>
+    <col min="30" max="41" width="3.83203125" style="14" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -36051,23 +36077,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BP42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
+    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="BL48" sqref="BL48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="12"/>
-    <col min="2" max="3" width="3.765625" style="12" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" style="13" customWidth="1"/>
-    <col min="16" max="16" width="9.14453125" style="12" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" style="12" customWidth="1"/>
-    <col min="29" max="29" width="9.14453125" style="12"/>
-    <col min="30" max="41" width="3.8984375" style="12" customWidth="1"/>
-    <col min="42" max="16384" width="9.14453125" style="12"/>
+    <col min="1" max="1" width="9.1640625" style="12"/>
+    <col min="2" max="3" width="3.83203125" style="12" customWidth="1"/>
+    <col min="4" max="15" width="3.83203125" style="13" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="12" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" style="12" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="12"/>
+    <col min="30" max="41" width="3.83203125" style="12" customWidth="1"/>
+    <col min="42" max="16384" width="9.1640625" style="12"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:68" x14ac:dyDescent="0.2">
@@ -40551,297 +40577,293 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A2:EF121"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:EF121"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="40" zoomScaleNormal="40" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
-      <selection activeCell="EB58" sqref="EB58"/>
+    <sheetView tabSelected="1" zoomScale="47" zoomScaleNormal="47" zoomScalePageLayoutView="47" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5:AO13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.14453125" style="16"/>
-    <col min="2" max="2" width="4.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="3.765625" customWidth="1"/>
-    <col min="4" max="15" width="3.8984375" customWidth="1"/>
-    <col min="17" max="28" width="3.8984375" customWidth="1"/>
-    <col min="30" max="41" width="3.8984375" customWidth="1"/>
-    <col min="42" max="42" width="9.14453125" style="16"/>
-    <col min="43" max="43" width="4.5703125" style="16" customWidth="1"/>
-    <col min="44" max="44" width="3.765625" style="16" customWidth="1"/>
-    <col min="45" max="52" width="3.8984375" style="16" customWidth="1"/>
-    <col min="53" max="56" width="3.8984375" customWidth="1"/>
-    <col min="58" max="69" width="3.8984375" customWidth="1"/>
-    <col min="71" max="82" width="3.8984375" customWidth="1"/>
-    <col min="84" max="84" width="4.5703125" customWidth="1"/>
-    <col min="85" max="85" width="3.765625" customWidth="1"/>
-    <col min="86" max="97" width="3.8984375" customWidth="1"/>
-    <col min="99" max="110" width="3.8984375" customWidth="1"/>
-    <col min="112" max="123" width="3.8984375" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="16" customWidth="1"/>
+    <col min="3" max="15" width="3.83203125" customWidth="1"/>
+    <col min="17" max="28" width="3.83203125" customWidth="1"/>
+    <col min="30" max="41" width="3.83203125" customWidth="1"/>
+    <col min="42" max="42" width="8.83203125" style="16"/>
+    <col min="43" max="43" width="4.5" style="16" customWidth="1"/>
+    <col min="44" max="52" width="3.83203125" style="16" customWidth="1"/>
+    <col min="53" max="56" width="3.83203125" customWidth="1"/>
+    <col min="58" max="69" width="3.83203125" customWidth="1"/>
+    <col min="71" max="82" width="3.83203125" customWidth="1"/>
+    <col min="84" max="84" width="4.5" customWidth="1"/>
+    <col min="85" max="97" width="3.83203125" customWidth="1"/>
+    <col min="99" max="110" width="3.83203125" customWidth="1"/>
+    <col min="112" max="123" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:136" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:136" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="44" t="s">
+    <row r="3" spans="2:136" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="D3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="44"/>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="44"/>
-      <c r="AM3" s="44"/>
-      <c r="AN3" s="44"/>
-      <c r="AO3" s="44"/>
-      <c r="AS3" s="44" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="43"/>
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="43"/>
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="43"/>
+      <c r="AL3" s="43"/>
+      <c r="AM3" s="43"/>
+      <c r="AN3" s="43"/>
+      <c r="AO3" s="43"/>
+      <c r="AS3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="AT3" s="44"/>
-      <c r="AU3" s="44"/>
-      <c r="AV3" s="44"/>
-      <c r="AW3" s="44"/>
-      <c r="AX3" s="44"/>
-      <c r="AY3" s="44"/>
-      <c r="AZ3" s="44"/>
-      <c r="BA3" s="44"/>
-      <c r="BB3" s="44"/>
-      <c r="BC3" s="44"/>
-      <c r="BD3" s="44"/>
-      <c r="BE3" s="44"/>
-      <c r="BF3" s="44"/>
-      <c r="BG3" s="44"/>
-      <c r="BH3" s="44"/>
-      <c r="BI3" s="44"/>
-      <c r="BJ3" s="44"/>
-      <c r="BK3" s="44"/>
-      <c r="BL3" s="44"/>
-      <c r="BM3" s="44"/>
-      <c r="BN3" s="44"/>
-      <c r="BO3" s="44"/>
-      <c r="BP3" s="44"/>
-      <c r="BQ3" s="44"/>
-      <c r="BR3" s="44"/>
-      <c r="BS3" s="44"/>
-      <c r="BT3" s="44"/>
-      <c r="BU3" s="44"/>
-      <c r="BV3" s="44"/>
-      <c r="BW3" s="44"/>
-      <c r="BX3" s="44"/>
-      <c r="BY3" s="44"/>
-      <c r="BZ3" s="44"/>
-      <c r="CA3" s="44"/>
-      <c r="CB3" s="44"/>
-      <c r="CC3" s="44"/>
-      <c r="CD3" s="44"/>
-      <c r="CH3" s="44" t="s">
+      <c r="AT3" s="43"/>
+      <c r="AU3" s="43"/>
+      <c r="AV3" s="43"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="43"/>
+      <c r="AY3" s="43"/>
+      <c r="AZ3" s="43"/>
+      <c r="BA3" s="43"/>
+      <c r="BB3" s="43"/>
+      <c r="BC3" s="43"/>
+      <c r="BD3" s="43"/>
+      <c r="BE3" s="43"/>
+      <c r="BF3" s="43"/>
+      <c r="BG3" s="43"/>
+      <c r="BH3" s="43"/>
+      <c r="BI3" s="43"/>
+      <c r="BJ3" s="43"/>
+      <c r="BK3" s="43"/>
+      <c r="BL3" s="43"/>
+      <c r="BM3" s="43"/>
+      <c r="BN3" s="43"/>
+      <c r="BO3" s="43"/>
+      <c r="BP3" s="43"/>
+      <c r="BQ3" s="43"/>
+      <c r="BR3" s="43"/>
+      <c r="BS3" s="43"/>
+      <c r="BT3" s="43"/>
+      <c r="BU3" s="43"/>
+      <c r="BV3" s="43"/>
+      <c r="BW3" s="43"/>
+      <c r="BX3" s="43"/>
+      <c r="BY3" s="43"/>
+      <c r="BZ3" s="43"/>
+      <c r="CA3" s="43"/>
+      <c r="CB3" s="43"/>
+      <c r="CC3" s="43"/>
+      <c r="CD3" s="43"/>
+      <c r="CH3" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="CI3" s="44"/>
-      <c r="CJ3" s="44"/>
-      <c r="CK3" s="44"/>
-      <c r="CL3" s="44"/>
-      <c r="CM3" s="44"/>
-      <c r="CN3" s="44"/>
-      <c r="CO3" s="44"/>
-      <c r="CP3" s="44"/>
-      <c r="CQ3" s="44"/>
-      <c r="CR3" s="44"/>
-      <c r="CS3" s="44"/>
-      <c r="CT3" s="44"/>
-      <c r="CU3" s="44"/>
-      <c r="CV3" s="44"/>
-      <c r="CW3" s="44"/>
-      <c r="CX3" s="44"/>
-      <c r="CY3" s="44"/>
-      <c r="CZ3" s="44"/>
-      <c r="DA3" s="44"/>
-      <c r="DB3" s="44"/>
-      <c r="DC3" s="44"/>
-      <c r="DD3" s="44"/>
-      <c r="DE3" s="44"/>
-      <c r="DF3" s="44"/>
-      <c r="DG3" s="44"/>
-      <c r="DH3" s="44"/>
-      <c r="DI3" s="44"/>
-      <c r="DJ3" s="44"/>
-      <c r="DK3" s="44"/>
-      <c r="DL3" s="44"/>
-      <c r="DM3" s="44"/>
-      <c r="DN3" s="44"/>
-      <c r="DO3" s="44"/>
-      <c r="DP3" s="44"/>
-      <c r="DQ3" s="44"/>
-      <c r="DR3" s="44"/>
-      <c r="DS3" s="44"/>
+      <c r="CI3" s="43"/>
+      <c r="CJ3" s="43"/>
+      <c r="CK3" s="43"/>
+      <c r="CL3" s="43"/>
+      <c r="CM3" s="43"/>
+      <c r="CN3" s="43"/>
+      <c r="CO3" s="43"/>
+      <c r="CP3" s="43"/>
+      <c r="CQ3" s="43"/>
+      <c r="CR3" s="43"/>
+      <c r="CS3" s="43"/>
+      <c r="CT3" s="43"/>
+      <c r="CU3" s="43"/>
+      <c r="CV3" s="43"/>
+      <c r="CW3" s="43"/>
+      <c r="CX3" s="43"/>
+      <c r="CY3" s="43"/>
+      <c r="CZ3" s="43"/>
+      <c r="DA3" s="43"/>
+      <c r="DB3" s="43"/>
+      <c r="DC3" s="43"/>
+      <c r="DD3" s="43"/>
+      <c r="DE3" s="43"/>
+      <c r="DF3" s="43"/>
+      <c r="DG3" s="43"/>
+      <c r="DH3" s="43"/>
+      <c r="DI3" s="43"/>
+      <c r="DJ3" s="43"/>
+      <c r="DK3" s="43"/>
+      <c r="DL3" s="43"/>
+      <c r="DM3" s="43"/>
+      <c r="DN3" s="43"/>
+      <c r="DO3" s="43"/>
+      <c r="DP3" s="43"/>
+      <c r="DQ3" s="43"/>
+      <c r="DR3" s="43"/>
+      <c r="DS3" s="43"/>
     </row>
-    <row r="4" spans="2:136" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:136" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
       <c r="P4" s="19"/>
-      <c r="Q4" s="43" t="s">
+      <c r="Q4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
       <c r="AC4" s="19"/>
-      <c r="AD4" s="43" t="s">
+      <c r="AD4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="43"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="43"/>
-      <c r="AK4" s="43"/>
-      <c r="AL4" s="43"/>
-      <c r="AM4" s="43"/>
-      <c r="AN4" s="43"/>
-      <c r="AO4" s="43"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="44"/>
+      <c r="AH4" s="44"/>
+      <c r="AI4" s="44"/>
+      <c r="AJ4" s="44"/>
+      <c r="AK4" s="44"/>
+      <c r="AL4" s="44"/>
+      <c r="AM4" s="44"/>
+      <c r="AN4" s="44"/>
+      <c r="AO4" s="44"/>
       <c r="AQ4" s="41"/>
       <c r="AR4" s="41"/>
-      <c r="AS4" s="43" t="s">
+      <c r="AS4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="AT4" s="43"/>
-      <c r="AU4" s="43"/>
-      <c r="AV4" s="43"/>
-      <c r="AW4" s="43"/>
-      <c r="AX4" s="43"/>
-      <c r="AY4" s="43"/>
-      <c r="AZ4" s="43"/>
-      <c r="BA4" s="43"/>
-      <c r="BB4" s="43"/>
-      <c r="BC4" s="43"/>
-      <c r="BD4" s="43"/>
+      <c r="AT4" s="44"/>
+      <c r="AU4" s="44"/>
+      <c r="AV4" s="44"/>
+      <c r="AW4" s="44"/>
+      <c r="AX4" s="44"/>
+      <c r="AY4" s="44"/>
+      <c r="AZ4" s="44"/>
+      <c r="BA4" s="44"/>
+      <c r="BB4" s="44"/>
+      <c r="BC4" s="44"/>
+      <c r="BD4" s="44"/>
       <c r="BE4" s="19"/>
-      <c r="BF4" s="43" t="s">
+      <c r="BF4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BG4" s="43"/>
-      <c r="BH4" s="43"/>
-      <c r="BI4" s="43"/>
-      <c r="BJ4" s="43"/>
-      <c r="BK4" s="43"/>
-      <c r="BL4" s="43"/>
-      <c r="BM4" s="43"/>
-      <c r="BN4" s="43"/>
-      <c r="BO4" s="43"/>
-      <c r="BP4" s="43"/>
-      <c r="BQ4" s="43"/>
+      <c r="BG4" s="44"/>
+      <c r="BH4" s="44"/>
+      <c r="BI4" s="44"/>
+      <c r="BJ4" s="44"/>
+      <c r="BK4" s="44"/>
+      <c r="BL4" s="44"/>
+      <c r="BM4" s="44"/>
+      <c r="BN4" s="44"/>
+      <c r="BO4" s="44"/>
+      <c r="BP4" s="44"/>
+      <c r="BQ4" s="44"/>
       <c r="BR4" s="19"/>
-      <c r="BS4" s="43" t="s">
+      <c r="BS4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="BT4" s="43"/>
-      <c r="BU4" s="43"/>
-      <c r="BV4" s="43"/>
-      <c r="BW4" s="43"/>
-      <c r="BX4" s="43"/>
-      <c r="BY4" s="43"/>
-      <c r="BZ4" s="43"/>
-      <c r="CA4" s="43"/>
-      <c r="CB4" s="43"/>
-      <c r="CC4" s="43"/>
-      <c r="CD4" s="43"/>
+      <c r="BT4" s="44"/>
+      <c r="BU4" s="44"/>
+      <c r="BV4" s="44"/>
+      <c r="BW4" s="44"/>
+      <c r="BX4" s="44"/>
+      <c r="BY4" s="44"/>
+      <c r="BZ4" s="44"/>
+      <c r="CA4" s="44"/>
+      <c r="CB4" s="44"/>
+      <c r="CC4" s="44"/>
+      <c r="CD4" s="44"/>
       <c r="CF4" s="41"/>
       <c r="CG4" s="41"/>
-      <c r="CH4" s="43" t="s">
+      <c r="CH4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="CI4" s="43"/>
-      <c r="CJ4" s="43"/>
-      <c r="CK4" s="43"/>
-      <c r="CL4" s="43"/>
-      <c r="CM4" s="43"/>
-      <c r="CN4" s="43"/>
-      <c r="CO4" s="43"/>
-      <c r="CP4" s="43"/>
-      <c r="CQ4" s="43"/>
-      <c r="CR4" s="43"/>
-      <c r="CS4" s="43"/>
+      <c r="CI4" s="44"/>
+      <c r="CJ4" s="44"/>
+      <c r="CK4" s="44"/>
+      <c r="CL4" s="44"/>
+      <c r="CM4" s="44"/>
+      <c r="CN4" s="44"/>
+      <c r="CO4" s="44"/>
+      <c r="CP4" s="44"/>
+      <c r="CQ4" s="44"/>
+      <c r="CR4" s="44"/>
+      <c r="CS4" s="44"/>
       <c r="CT4" s="19"/>
-      <c r="CU4" s="43" t="s">
+      <c r="CU4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="CV4" s="43"/>
-      <c r="CW4" s="43"/>
-      <c r="CX4" s="43"/>
-      <c r="CY4" s="43"/>
-      <c r="CZ4" s="43"/>
-      <c r="DA4" s="43"/>
-      <c r="DB4" s="43"/>
-      <c r="DC4" s="43"/>
-      <c r="DD4" s="43"/>
-      <c r="DE4" s="43"/>
-      <c r="DF4" s="43"/>
+      <c r="CV4" s="44"/>
+      <c r="CW4" s="44"/>
+      <c r="CX4" s="44"/>
+      <c r="CY4" s="44"/>
+      <c r="CZ4" s="44"/>
+      <c r="DA4" s="44"/>
+      <c r="DB4" s="44"/>
+      <c r="DC4" s="44"/>
+      <c r="DD4" s="44"/>
+      <c r="DE4" s="44"/>
+      <c r="DF4" s="44"/>
       <c r="DG4" s="19"/>
-      <c r="DH4" s="43" t="s">
+      <c r="DH4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="DI4" s="43"/>
-      <c r="DJ4" s="43"/>
-      <c r="DK4" s="43"/>
-      <c r="DL4" s="43"/>
-      <c r="DM4" s="43"/>
-      <c r="DN4" s="43"/>
-      <c r="DO4" s="43"/>
-      <c r="DP4" s="43"/>
-      <c r="DQ4" s="43"/>
-      <c r="DR4" s="43"/>
-      <c r="DS4" s="43"/>
+      <c r="DI4" s="44"/>
+      <c r="DJ4" s="44"/>
+      <c r="DK4" s="44"/>
+      <c r="DL4" s="44"/>
+      <c r="DM4" s="44"/>
+      <c r="DN4" s="44"/>
+      <c r="DO4" s="44"/>
+      <c r="DP4" s="44"/>
+      <c r="DQ4" s="44"/>
+      <c r="DR4" s="44"/>
+      <c r="DS4" s="44"/>
       <c r="DW4" s="17" t="s">
         <v>7</v>
       </c>
@@ -42846,157 +42868,157 @@
       <c r="EE17"/>
       <c r="EF17"/>
     </row>
-    <row r="18" spans="2:136" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:136" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="42" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
       <c r="P18" s="19"/>
-      <c r="Q18" s="43" t="s">
+      <c r="Q18" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="43"/>
-      <c r="AB18" s="43"/>
+      <c r="R18" s="44"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="44"/>
+      <c r="W18" s="44"/>
+      <c r="X18" s="44"/>
+      <c r="Y18" s="44"/>
+      <c r="Z18" s="44"/>
+      <c r="AA18" s="44"/>
+      <c r="AB18" s="44"/>
       <c r="AC18" s="19"/>
-      <c r="AD18" s="43" t="s">
+      <c r="AD18" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AE18" s="43"/>
-      <c r="AF18" s="43"/>
-      <c r="AG18" s="43"/>
-      <c r="AH18" s="43"/>
-      <c r="AI18" s="43"/>
-      <c r="AJ18" s="43"/>
-      <c r="AK18" s="43"/>
-      <c r="AL18" s="43"/>
-      <c r="AM18" s="43"/>
-      <c r="AN18" s="43"/>
-      <c r="AO18" s="43"/>
+      <c r="AE18" s="44"/>
+      <c r="AF18" s="44"/>
+      <c r="AG18" s="44"/>
+      <c r="AH18" s="44"/>
+      <c r="AI18" s="44"/>
+      <c r="AJ18" s="44"/>
+      <c r="AK18" s="44"/>
+      <c r="AL18" s="44"/>
+      <c r="AM18" s="44"/>
+      <c r="AN18" s="44"/>
+      <c r="AO18" s="44"/>
       <c r="AQ18" s="42" t="s">
         <v>15</v>
       </c>
       <c r="AR18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AS18" s="43" t="s">
+      <c r="AS18" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="AT18" s="43"/>
-      <c r="AU18" s="43"/>
-      <c r="AV18" s="43"/>
-      <c r="AW18" s="43"/>
-      <c r="AX18" s="43"/>
-      <c r="AY18" s="43"/>
-      <c r="AZ18" s="43"/>
-      <c r="BA18" s="43"/>
-      <c r="BB18" s="43"/>
-      <c r="BC18" s="43"/>
-      <c r="BD18" s="43"/>
+      <c r="AT18" s="44"/>
+      <c r="AU18" s="44"/>
+      <c r="AV18" s="44"/>
+      <c r="AW18" s="44"/>
+      <c r="AX18" s="44"/>
+      <c r="AY18" s="44"/>
+      <c r="AZ18" s="44"/>
+      <c r="BA18" s="44"/>
+      <c r="BB18" s="44"/>
+      <c r="BC18" s="44"/>
+      <c r="BD18" s="44"/>
       <c r="BE18" s="19"/>
-      <c r="BF18" s="43" t="s">
+      <c r="BF18" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="BG18" s="43"/>
-      <c r="BH18" s="43"/>
-      <c r="BI18" s="43"/>
-      <c r="BJ18" s="43"/>
-      <c r="BK18" s="43"/>
-      <c r="BL18" s="43"/>
-      <c r="BM18" s="43"/>
-      <c r="BN18" s="43"/>
-      <c r="BO18" s="43"/>
-      <c r="BP18" s="43"/>
-      <c r="BQ18" s="43"/>
+      <c r="BG18" s="44"/>
+      <c r="BH18" s="44"/>
+      <c r="BI18" s="44"/>
+      <c r="BJ18" s="44"/>
+      <c r="BK18" s="44"/>
+      <c r="BL18" s="44"/>
+      <c r="BM18" s="44"/>
+      <c r="BN18" s="44"/>
+      <c r="BO18" s="44"/>
+      <c r="BP18" s="44"/>
+      <c r="BQ18" s="44"/>
       <c r="BR18" s="19"/>
-      <c r="BS18" s="43" t="s">
+      <c r="BS18" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="BT18" s="43"/>
-      <c r="BU18" s="43"/>
-      <c r="BV18" s="43"/>
-      <c r="BW18" s="43"/>
-      <c r="BX18" s="43"/>
-      <c r="BY18" s="43"/>
-      <c r="BZ18" s="43"/>
-      <c r="CA18" s="43"/>
-      <c r="CB18" s="43"/>
-      <c r="CC18" s="43"/>
-      <c r="CD18" s="43"/>
+      <c r="BT18" s="44"/>
+      <c r="BU18" s="44"/>
+      <c r="BV18" s="44"/>
+      <c r="BW18" s="44"/>
+      <c r="BX18" s="44"/>
+      <c r="BY18" s="44"/>
+      <c r="BZ18" s="44"/>
+      <c r="CA18" s="44"/>
+      <c r="CB18" s="44"/>
+      <c r="CC18" s="44"/>
+      <c r="CD18" s="44"/>
       <c r="CF18" s="42" t="s">
         <v>17</v>
       </c>
       <c r="CG18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="CH18" s="43" t="s">
+      <c r="CH18" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="CI18" s="43"/>
-      <c r="CJ18" s="43"/>
-      <c r="CK18" s="43"/>
-      <c r="CL18" s="43"/>
-      <c r="CM18" s="43"/>
-      <c r="CN18" s="43"/>
-      <c r="CO18" s="43"/>
-      <c r="CP18" s="43"/>
-      <c r="CQ18" s="43"/>
-      <c r="CR18" s="43"/>
-      <c r="CS18" s="43"/>
+      <c r="CI18" s="44"/>
+      <c r="CJ18" s="44"/>
+      <c r="CK18" s="44"/>
+      <c r="CL18" s="44"/>
+      <c r="CM18" s="44"/>
+      <c r="CN18" s="44"/>
+      <c r="CO18" s="44"/>
+      <c r="CP18" s="44"/>
+      <c r="CQ18" s="44"/>
+      <c r="CR18" s="44"/>
+      <c r="CS18" s="44"/>
       <c r="CT18" s="19"/>
-      <c r="CU18" s="43" t="s">
+      <c r="CU18" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="CV18" s="43"/>
-      <c r="CW18" s="43"/>
-      <c r="CX18" s="43"/>
-      <c r="CY18" s="43"/>
-      <c r="CZ18" s="43"/>
-      <c r="DA18" s="43"/>
-      <c r="DB18" s="43"/>
-      <c r="DC18" s="43"/>
-      <c r="DD18" s="43"/>
-      <c r="DE18" s="43"/>
-      <c r="DF18" s="43"/>
+      <c r="CV18" s="44"/>
+      <c r="CW18" s="44"/>
+      <c r="CX18" s="44"/>
+      <c r="CY18" s="44"/>
+      <c r="CZ18" s="44"/>
+      <c r="DA18" s="44"/>
+      <c r="DB18" s="44"/>
+      <c r="DC18" s="44"/>
+      <c r="DD18" s="44"/>
+      <c r="DE18" s="44"/>
+      <c r="DF18" s="44"/>
       <c r="DG18" s="19"/>
-      <c r="DH18" s="43" t="s">
+      <c r="DH18" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="DI18" s="43"/>
-      <c r="DJ18" s="43"/>
-      <c r="DK18" s="43"/>
-      <c r="DL18" s="43"/>
-      <c r="DM18" s="43"/>
-      <c r="DN18" s="43"/>
-      <c r="DO18" s="43"/>
-      <c r="DP18" s="43"/>
-      <c r="DQ18" s="43"/>
-      <c r="DR18" s="43"/>
-      <c r="DS18" s="43"/>
+      <c r="DI18" s="44"/>
+      <c r="DJ18" s="44"/>
+      <c r="DK18" s="44"/>
+      <c r="DL18" s="44"/>
+      <c r="DM18" s="44"/>
+      <c r="DN18" s="44"/>
+      <c r="DO18" s="44"/>
+      <c r="DP18" s="44"/>
+      <c r="DQ18" s="44"/>
+      <c r="DR18" s="44"/>
+      <c r="DS18" s="44"/>
     </row>
     <row r="19" spans="2:136" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="42"/>
@@ -73341,17 +73363,166 @@
     </row>
   </sheetData>
   <mergeCells count="195">
-    <mergeCell ref="AD11:AO11"/>
-    <mergeCell ref="AD12:AO12"/>
-    <mergeCell ref="AD13:AO13"/>
-    <mergeCell ref="Q7:AB7"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:O15"/>
-    <mergeCell ref="Q15:AB15"/>
-    <mergeCell ref="AD15:AO15"/>
-    <mergeCell ref="AS15:BD15"/>
-    <mergeCell ref="AQ15:AR15"/>
-    <mergeCell ref="AS7:BD7"/>
+    <mergeCell ref="CF18:CF121"/>
+    <mergeCell ref="CH18:CS18"/>
+    <mergeCell ref="CU18:DF18"/>
+    <mergeCell ref="DH18:DS18"/>
+    <mergeCell ref="CG19:CG30"/>
+    <mergeCell ref="CG32:CG43"/>
+    <mergeCell ref="CG45:CG56"/>
+    <mergeCell ref="CG58:CG69"/>
+    <mergeCell ref="CG71:CG82"/>
+    <mergeCell ref="CG84:CG95"/>
+    <mergeCell ref="CG97:CG108"/>
+    <mergeCell ref="CG110:CG121"/>
+    <mergeCell ref="CF14:CG14"/>
+    <mergeCell ref="CH14:CS14"/>
+    <mergeCell ref="CU14:DF14"/>
+    <mergeCell ref="DH14:DS14"/>
+    <mergeCell ref="CF16:CG16"/>
+    <mergeCell ref="CH16:CS16"/>
+    <mergeCell ref="CU16:DF16"/>
+    <mergeCell ref="DH16:DS16"/>
+    <mergeCell ref="CF12:CG12"/>
+    <mergeCell ref="CH12:CS12"/>
+    <mergeCell ref="CU12:DF12"/>
+    <mergeCell ref="DH12:DS12"/>
+    <mergeCell ref="CF13:CG13"/>
+    <mergeCell ref="CH13:CS13"/>
+    <mergeCell ref="CU13:DF13"/>
+    <mergeCell ref="DH13:DS13"/>
+    <mergeCell ref="DH15:DS15"/>
+    <mergeCell ref="CH15:CS15"/>
+    <mergeCell ref="CU15:DF15"/>
+    <mergeCell ref="CF15:CG15"/>
+    <mergeCell ref="CF10:CG10"/>
+    <mergeCell ref="CH10:CS10"/>
+    <mergeCell ref="CU10:DF10"/>
+    <mergeCell ref="DH10:DS10"/>
+    <mergeCell ref="CF11:CG11"/>
+    <mergeCell ref="CH11:CS11"/>
+    <mergeCell ref="CU11:DF11"/>
+    <mergeCell ref="DH11:DS11"/>
+    <mergeCell ref="CF8:CG8"/>
+    <mergeCell ref="CH8:CS8"/>
+    <mergeCell ref="CU8:DF8"/>
+    <mergeCell ref="DH8:DS8"/>
+    <mergeCell ref="CF9:CG9"/>
+    <mergeCell ref="CH9:CS9"/>
+    <mergeCell ref="CU9:DF9"/>
+    <mergeCell ref="DH9:DS9"/>
+    <mergeCell ref="DH6:DS6"/>
+    <mergeCell ref="CF7:CG7"/>
+    <mergeCell ref="CH7:CS7"/>
+    <mergeCell ref="CU7:DF7"/>
+    <mergeCell ref="DH7:DS7"/>
+    <mergeCell ref="AQ16:AR16"/>
+    <mergeCell ref="AS16:BD16"/>
+    <mergeCell ref="BF16:BQ16"/>
+    <mergeCell ref="BS16:CD16"/>
+    <mergeCell ref="CF6:CG6"/>
+    <mergeCell ref="CH6:CS6"/>
+    <mergeCell ref="CU6:DF6"/>
+    <mergeCell ref="AQ13:AR13"/>
+    <mergeCell ref="AS13:BD13"/>
+    <mergeCell ref="BF13:BQ13"/>
+    <mergeCell ref="BS13:CD13"/>
+    <mergeCell ref="AQ14:AR14"/>
+    <mergeCell ref="AS14:BD14"/>
+    <mergeCell ref="BF14:BQ14"/>
+    <mergeCell ref="BS14:CD14"/>
+    <mergeCell ref="AQ11:AR11"/>
+    <mergeCell ref="AS11:BD11"/>
+    <mergeCell ref="BF11:BQ11"/>
+    <mergeCell ref="BS11:CD11"/>
+    <mergeCell ref="CH3:DS3"/>
+    <mergeCell ref="CF4:CG4"/>
+    <mergeCell ref="CH4:CS4"/>
+    <mergeCell ref="CU4:DF4"/>
+    <mergeCell ref="DH4:DS4"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CH5:CS5"/>
+    <mergeCell ref="CU5:DF5"/>
+    <mergeCell ref="DH5:DS5"/>
+    <mergeCell ref="BF7:BQ7"/>
+    <mergeCell ref="BS7:CD7"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AS8:BD8"/>
+    <mergeCell ref="BF8:BQ8"/>
+    <mergeCell ref="BS8:CD8"/>
+    <mergeCell ref="AR97:AR108"/>
+    <mergeCell ref="AR110:AR121"/>
+    <mergeCell ref="AQ12:AR12"/>
+    <mergeCell ref="AS12:BD12"/>
+    <mergeCell ref="BF12:BQ12"/>
+    <mergeCell ref="BS12:CD12"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="AS9:BD9"/>
+    <mergeCell ref="BF9:BQ9"/>
+    <mergeCell ref="BS9:CD9"/>
+    <mergeCell ref="AQ10:AR10"/>
+    <mergeCell ref="AS10:BD10"/>
+    <mergeCell ref="BF10:BQ10"/>
+    <mergeCell ref="BS10:CD10"/>
+    <mergeCell ref="BF15:BQ15"/>
+    <mergeCell ref="BS15:CD15"/>
+    <mergeCell ref="AS3:CD3"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AS4:BD4"/>
+    <mergeCell ref="BF4:BQ4"/>
+    <mergeCell ref="BS4:CD4"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AS5:BD5"/>
+    <mergeCell ref="BF5:BQ5"/>
+    <mergeCell ref="BS5:CD5"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AS6:BD6"/>
+    <mergeCell ref="BF6:BQ6"/>
+    <mergeCell ref="BS6:CD6"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AS18:BD18"/>
+    <mergeCell ref="BF18:BQ18"/>
+    <mergeCell ref="BS18:CD18"/>
+    <mergeCell ref="C110:C121"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="Q13:AB13"/>
+    <mergeCell ref="D16:O16"/>
+    <mergeCell ref="C97:C108"/>
+    <mergeCell ref="D18:O18"/>
+    <mergeCell ref="Q18:AB18"/>
+    <mergeCell ref="AD18:AO18"/>
+    <mergeCell ref="C19:C30"/>
+    <mergeCell ref="C32:C43"/>
+    <mergeCell ref="C45:C56"/>
+    <mergeCell ref="C58:C69"/>
+    <mergeCell ref="C71:C82"/>
+    <mergeCell ref="C84:C95"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="Q14:AB14"/>
+    <mergeCell ref="Q16:AB16"/>
+    <mergeCell ref="AD14:AO14"/>
+    <mergeCell ref="AD16:AO16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:O9"/>
+    <mergeCell ref="Q9:AB9"/>
+    <mergeCell ref="AD9:AO9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="Q8:AB8"/>
+    <mergeCell ref="Q10:AB10"/>
+    <mergeCell ref="Q11:AB11"/>
+    <mergeCell ref="Q12:AB12"/>
+    <mergeCell ref="AD6:AO6"/>
+    <mergeCell ref="AD7:AO7"/>
+    <mergeCell ref="AD8:AO8"/>
+    <mergeCell ref="AD10:AO10"/>
     <mergeCell ref="B18:B121"/>
     <mergeCell ref="AQ18:AQ121"/>
     <mergeCell ref="AR19:AR30"/>
@@ -73376,166 +73547,17 @@
     <mergeCell ref="D10:O10"/>
     <mergeCell ref="D4:O4"/>
     <mergeCell ref="AD5:AO5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="Q14:AB14"/>
-    <mergeCell ref="Q16:AB16"/>
-    <mergeCell ref="AD14:AO14"/>
-    <mergeCell ref="AD16:AO16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:O9"/>
-    <mergeCell ref="Q9:AB9"/>
-    <mergeCell ref="AD9:AO9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="Q8:AB8"/>
-    <mergeCell ref="Q10:AB10"/>
-    <mergeCell ref="Q11:AB11"/>
-    <mergeCell ref="Q12:AB12"/>
-    <mergeCell ref="AD6:AO6"/>
-    <mergeCell ref="AD7:AO7"/>
-    <mergeCell ref="AD8:AO8"/>
-    <mergeCell ref="AD10:AO10"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AS6:BD6"/>
-    <mergeCell ref="BF6:BQ6"/>
-    <mergeCell ref="BS6:CD6"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AS18:BD18"/>
-    <mergeCell ref="BF18:BQ18"/>
-    <mergeCell ref="BS18:CD18"/>
-    <mergeCell ref="C110:C121"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="Q13:AB13"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="C97:C108"/>
-    <mergeCell ref="D18:O18"/>
-    <mergeCell ref="Q18:AB18"/>
-    <mergeCell ref="AD18:AO18"/>
-    <mergeCell ref="C19:C30"/>
-    <mergeCell ref="C32:C43"/>
-    <mergeCell ref="C45:C56"/>
-    <mergeCell ref="C58:C69"/>
-    <mergeCell ref="C71:C82"/>
-    <mergeCell ref="C84:C95"/>
-    <mergeCell ref="AS3:CD3"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AS4:BD4"/>
-    <mergeCell ref="BF4:BQ4"/>
-    <mergeCell ref="BS4:CD4"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AS5:BD5"/>
-    <mergeCell ref="BF5:BQ5"/>
-    <mergeCell ref="BS5:CD5"/>
-    <mergeCell ref="BF7:BQ7"/>
-    <mergeCell ref="BS7:CD7"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AS8:BD8"/>
-    <mergeCell ref="BF8:BQ8"/>
-    <mergeCell ref="BS8:CD8"/>
-    <mergeCell ref="AR97:AR108"/>
-    <mergeCell ref="AR110:AR121"/>
-    <mergeCell ref="AQ12:AR12"/>
-    <mergeCell ref="AS12:BD12"/>
-    <mergeCell ref="BF12:BQ12"/>
-    <mergeCell ref="BS12:CD12"/>
-    <mergeCell ref="AQ9:AR9"/>
-    <mergeCell ref="AS9:BD9"/>
-    <mergeCell ref="BF9:BQ9"/>
-    <mergeCell ref="BS9:CD9"/>
-    <mergeCell ref="AQ10:AR10"/>
-    <mergeCell ref="AS10:BD10"/>
-    <mergeCell ref="BF10:BQ10"/>
-    <mergeCell ref="BS10:CD10"/>
-    <mergeCell ref="BF15:BQ15"/>
-    <mergeCell ref="BS15:CD15"/>
-    <mergeCell ref="CH3:DS3"/>
-    <mergeCell ref="CF4:CG4"/>
-    <mergeCell ref="CH4:CS4"/>
-    <mergeCell ref="CU4:DF4"/>
-    <mergeCell ref="DH4:DS4"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CH5:CS5"/>
-    <mergeCell ref="CU5:DF5"/>
-    <mergeCell ref="DH5:DS5"/>
-    <mergeCell ref="DH6:DS6"/>
-    <mergeCell ref="CF7:CG7"/>
-    <mergeCell ref="CH7:CS7"/>
-    <mergeCell ref="CU7:DF7"/>
-    <mergeCell ref="DH7:DS7"/>
-    <mergeCell ref="AQ16:AR16"/>
-    <mergeCell ref="AS16:BD16"/>
-    <mergeCell ref="BF16:BQ16"/>
-    <mergeCell ref="BS16:CD16"/>
-    <mergeCell ref="CF6:CG6"/>
-    <mergeCell ref="CH6:CS6"/>
-    <mergeCell ref="CU6:DF6"/>
-    <mergeCell ref="AQ13:AR13"/>
-    <mergeCell ref="AS13:BD13"/>
-    <mergeCell ref="BF13:BQ13"/>
-    <mergeCell ref="BS13:CD13"/>
-    <mergeCell ref="AQ14:AR14"/>
-    <mergeCell ref="AS14:BD14"/>
-    <mergeCell ref="BF14:BQ14"/>
-    <mergeCell ref="BS14:CD14"/>
-    <mergeCell ref="AQ11:AR11"/>
-    <mergeCell ref="AS11:BD11"/>
-    <mergeCell ref="BF11:BQ11"/>
-    <mergeCell ref="BS11:CD11"/>
-    <mergeCell ref="CF10:CG10"/>
-    <mergeCell ref="CH10:CS10"/>
-    <mergeCell ref="CU10:DF10"/>
-    <mergeCell ref="DH10:DS10"/>
-    <mergeCell ref="CF11:CG11"/>
-    <mergeCell ref="CH11:CS11"/>
-    <mergeCell ref="CU11:DF11"/>
-    <mergeCell ref="DH11:DS11"/>
-    <mergeCell ref="CF8:CG8"/>
-    <mergeCell ref="CH8:CS8"/>
-    <mergeCell ref="CU8:DF8"/>
-    <mergeCell ref="DH8:DS8"/>
-    <mergeCell ref="CF9:CG9"/>
-    <mergeCell ref="CH9:CS9"/>
-    <mergeCell ref="CU9:DF9"/>
-    <mergeCell ref="DH9:DS9"/>
-    <mergeCell ref="CF14:CG14"/>
-    <mergeCell ref="CH14:CS14"/>
-    <mergeCell ref="CU14:DF14"/>
-    <mergeCell ref="DH14:DS14"/>
-    <mergeCell ref="CF16:CG16"/>
-    <mergeCell ref="CH16:CS16"/>
-    <mergeCell ref="CU16:DF16"/>
-    <mergeCell ref="DH16:DS16"/>
-    <mergeCell ref="CF12:CG12"/>
-    <mergeCell ref="CH12:CS12"/>
-    <mergeCell ref="CU12:DF12"/>
-    <mergeCell ref="DH12:DS12"/>
-    <mergeCell ref="CF13:CG13"/>
-    <mergeCell ref="CH13:CS13"/>
-    <mergeCell ref="CU13:DF13"/>
-    <mergeCell ref="DH13:DS13"/>
-    <mergeCell ref="DH15:DS15"/>
-    <mergeCell ref="CH15:CS15"/>
-    <mergeCell ref="CU15:DF15"/>
-    <mergeCell ref="CF15:CG15"/>
-    <mergeCell ref="CF18:CF121"/>
-    <mergeCell ref="CH18:CS18"/>
-    <mergeCell ref="CU18:DF18"/>
-    <mergeCell ref="DH18:DS18"/>
-    <mergeCell ref="CG19:CG30"/>
-    <mergeCell ref="CG32:CG43"/>
-    <mergeCell ref="CG45:CG56"/>
-    <mergeCell ref="CG58:CG69"/>
-    <mergeCell ref="CG71:CG82"/>
-    <mergeCell ref="CG84:CG95"/>
-    <mergeCell ref="CG97:CG108"/>
-    <mergeCell ref="CG110:CG121"/>
+    <mergeCell ref="AD11:AO11"/>
+    <mergeCell ref="AD12:AO12"/>
+    <mergeCell ref="AD13:AO13"/>
+    <mergeCell ref="Q7:AB7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:O15"/>
+    <mergeCell ref="Q15:AB15"/>
+    <mergeCell ref="AD15:AO15"/>
+    <mergeCell ref="AS15:BD15"/>
+    <mergeCell ref="AQ15:AR15"/>
+    <mergeCell ref="AS7:BD7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>